<commit_message>
repo2 asset2 bindcombo create copy improvment from bumbatproject
</commit_message>
<xml_diff>
--- a/ClearingFramework/functions/Гүйлгээ бүртгэх.xlsx
+++ b/ClearingFramework/functions/Гүйлгээ бүртгэх.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\Desktop\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\Documents\GitHub\ClearingFramework\ClearingFramework\functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87881F4F-539E-41E9-BE5F-77784EB8F004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57232C2-1AF7-4B6F-BB15-B0A503C99D30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31620" yWindow="2250" windowWidth="24585" windowHeight="12360" xr2:uid="{F35761CF-BBF5-47A2-933A-B47369EE1EF7}"/>
+    <workbookView xWindow="29190" yWindow="315" windowWidth="24585" windowHeight="12360" xr2:uid="{F35761CF-BBF5-47A2-933A-B47369EE1EF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +428,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>123</v>
+        <v>87979</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -445,7 +445,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>333</v>
+        <v>87980</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>123</v>
+        <v>87981</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -479,7 +479,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>333</v>
+        <v>87982</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>123</v>
+        <v>87983</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>333</v>
+        <v>87984</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>123</v>
+        <v>87985</v>
       </c>
       <c r="B8">
         <v>1</v>

</xml_diff>